<commit_message>
Testing performance changes on smaller model * Changed transforms tested to non-normalized values, no longer normalizing image, applying augment, then normalizing again * Updated weights of image * Set the 0 transform to None instead of having each transform's value as very low * Added in a default training_transform convertDataToLoaders(), made the dataloader for training have shuffle=True * Made a smaller model to evaluate differences easier between models, renamed the old resnet50classificaiton model to large2d * Updated to newer weights, much better performance (0.27 vs 0.49 for average accuracy for the small2D model, not that noticiable changes for large2d model) * No longer doing a train, val, test set. Now doing train and test set where val=test
</commit_message>
<xml_diff>
--- a/testResults.xlsx
+++ b/testResults.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnz\AppData\Local\Temp\Mxt241\RemoteFiles\1181214_2_33\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnz\AppData\Local\Temp\Mxt241\RemoteFiles\656804_3_18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0F580F-17FD-4928-9263-44F5B5BE1F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C26A2A-8BAC-4DBC-ABE7-A0D69204D3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6150" yWindow="1940" windowWidth="28800" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="475">
   <si>
     <t>name</t>
   </si>
@@ -1075,7 +1075,7 @@
     <t>no background tumor boxes adamw</t>
   </si>
   <si>
-    <t>testSamples24-7.py-batchSize=8-epochs=100-lr=0.001-evalDetailLine=no background tumor boxes adamw-hasBackground=f-usesLargestBox=f-segmentsMultiple=1-dropoutRate=0.2-grouped2D=f</t>
+    <t>testSamples24-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='no background tumor boxes adamw' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f</t>
   </si>
   <si>
     <t>{0: 4.4, 1: 6.4, 2: 6.2}</t>
@@ -1138,7 +1138,7 @@
     <t>background global boxes adamw</t>
   </si>
   <si>
-    <t>testSamples24-7.py-batchSize=8-epochs=100-lr=0.001-evalDetailLine=background global boxes adamw-hasBackground=t-usesLargestBox=t-segmentsMultiple=1-dropoutRate=0.2-grouped2D=f</t>
+    <t>testSamples24-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='background global boxes adamw' -hasBackground=t -usesLargestBox=t -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f</t>
   </si>
   <si>
     <t>{0: 3.8, 1: 7.6, 2: 5.6}</t>
@@ -1207,7 +1207,7 @@
     <t>background tumor boxes adamw</t>
   </si>
   <si>
-    <t>testSamples24-7.py-batchSize=8-epochs=100-lr=0.001-evalDetailLine=background tumor boxes adamw-hasBackground=t-usesLargestBox=f-segmentsMultiple=1-dropoutRate=0.2-grouped2D=f</t>
+    <t>testSamples24-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='background tumor boxes adamw' -hasBackground=t -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f</t>
   </si>
   <si>
     <t>{0: 2.8, 1: 9.8, 2: 4.4}</t>
@@ -1276,7 +1276,7 @@
     <t>no background global boxes adamw</t>
   </si>
   <si>
-    <t>testSamples24-7.py-batchSize=8-epochs=100-lr=0.001-evalDetailLine=no background global boxes adamw-hasBackground=f-usesLargestBox=t-segmentsMultiple=1-dropoutRate=0.2-grouped2D=f</t>
+    <t>testSamples24-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='no background global boxes adamw' -hasBackground=f -usesLargestBox=t -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f</t>
   </si>
   <si>
     <t>{0: 3.2, 1: 8.8, 2: 5.0}</t>
@@ -1337,6 +1337,114 @@
   </si>
   <si>
     <t>[4, 3, 3, 2, 2]</t>
+  </si>
+  <si>
+    <t>Weight tests, viewing performance of legacy vs new weights</t>
+  </si>
+  <si>
+    <t>legacy weights</t>
+  </si>
+  <si>
+    <t>Tests/0--/foldn5</t>
+  </si>
+  <si>
+    <t>python testSamples26-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='legacy weights' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Small2DResnet'</t>
+  </si>
+  <si>
+    <t>[None, None]</t>
+  </si>
+  <si>
+    <t>{0: 5.2, 1: 6.2, 2: 5.6}</t>
+  </si>
+  <si>
+    <t>[0.17647058823529413, 0.35294117647058826, 0.23529411764705882, 0.35294117647058826, 0.23529411764705882]</t>
+  </si>
+  <si>
+    <t>[0.20168067226890754, 0.3539467068878834, 0.2184873949579832, 0.3770053475935829, 0.23529411764705882]</t>
+  </si>
+  <si>
+    <t>[14, 11, 13, 15, 15]</t>
+  </si>
+  <si>
+    <t>newer weights</t>
+  </si>
+  <si>
+    <t>python testSamples26-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='newer weights' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Small2DResnet'</t>
+  </si>
+  <si>
+    <t>{0: 4.2, 1: 9.8, 2: 3.0}</t>
+  </si>
+  <si>
+    <t>[0.35294117647058826, 0.6470588235294118, 0.5294117647058824, 0.47058823529411764, 0.47058823529411764]</t>
+  </si>
+  <si>
+    <t>[0.3288613691090472, 0.6039215686274512, 0.5409753645047762, 0.36463708290333674, 0.44967320261437904]</t>
+  </si>
+  <si>
+    <t>[19, 25, 35, 17, 21]</t>
+  </si>
+  <si>
+    <t>python testSamples26-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='legacy weights' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Large2DResnet'</t>
+  </si>
+  <si>
+    <t>{0: 3.4, 1: 8.0, 2: 5.6}</t>
+  </si>
+  <si>
+    <t>[0.17647058823529413, 0.47058823529411764, 0.47058823529411764, 0.4117647058823529, 0.17647058823529413]</t>
+  </si>
+  <si>
+    <t>[0.17647058823529413, 0.492436974789916, 0.47058823529411764, 0.34506051224317474, 0.18137254901960784]</t>
+  </si>
+  <si>
+    <t>[15, 15, 16, 28, 11]</t>
+  </si>
+  <si>
+    <t>python testSamples26-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='newer weights' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Large2DResnet'</t>
+  </si>
+  <si>
+    <t>{0: 2.6, 1: 8.4, 2: 6.0}</t>
+  </si>
+  <si>
+    <t>[0.29411764705882354, 0.35294117647058826, 0.35294117647058826, 0.17647058823529413, 0.5294117647058824]</t>
+  </si>
+  <si>
+    <t>[0.273109243697479, 0.3025210084033613, 0.3740024681201152, 0.13003095975232196, 0.45940910300771887]</t>
+  </si>
+  <si>
+    <t>[17, 16, 18, 12, 22]</t>
+  </si>
+  <si>
+    <t>newer weights with padding same</t>
+  </si>
+  <si>
+    <t>newer weights with padding 0</t>
+  </si>
+  <si>
+    <t>python testSamples26-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='newer weights with padding 0' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Small2DResnet'</t>
+  </si>
+  <si>
+    <t>python testSamples26-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='newer weights with padding same' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Small2DResnet'</t>
+  </si>
+  <si>
+    <t>{0: 2.4, 1: 8.4, 2: 6.2}</t>
+  </si>
+  <si>
+    <t>[0.35294117647058826, 0.47058823529411764, 0.35294117647058826, 0.35294117647058826, 0.23529411764705882]</t>
+  </si>
+  <si>
+    <t>[0.3585434173669468, 0.4125632153313814, 0.35173453996983406, 0.28431372549019607, 0.23981900452488686]</t>
+  </si>
+  <si>
+    <t>[28, 24, 19, 23, 16]</t>
+  </si>
+  <si>
+    <t>newer weights with padding valid</t>
+  </si>
+  <si>
+    <t>python testSamples26-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='newer weights with padding valid' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Small2DResnet'</t>
+  </si>
+  <si>
+    <t>testing Padding on small model with tumor sizes (0 and valid padding seems to perform the same</t>
   </si>
 </sst>
 </file>
@@ -1676,10 +1784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y135"/>
+  <dimension ref="A1:Y154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="I137" sqref="I137"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9437,6 +9545,485 @@
         <v>438</v>
       </c>
     </row>
+    <row r="138" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="139" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="140" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>441</v>
+      </c>
+      <c r="B140">
+        <v>100</v>
+      </c>
+      <c r="C140">
+        <v>8</v>
+      </c>
+      <c r="D140">
+        <v>1E-3</v>
+      </c>
+      <c r="E140">
+        <v>0.2</v>
+      </c>
+      <c r="F140">
+        <v>0.01</v>
+      </c>
+      <c r="G140" t="s">
+        <v>442</v>
+      </c>
+      <c r="I140" t="s">
+        <v>443</v>
+      </c>
+      <c r="L140" t="s">
+        <v>443</v>
+      </c>
+      <c r="O140" t="s">
+        <v>444</v>
+      </c>
+      <c r="P140">
+        <v>0.27058823529411768</v>
+      </c>
+      <c r="Q140">
+        <v>0.2772828478710832</v>
+      </c>
+      <c r="R140">
+        <v>0.27058823529411768</v>
+      </c>
+      <c r="S140">
+        <v>9.7992180183451724E-2</v>
+      </c>
+      <c r="T140">
+        <v>0.1015540959098514</v>
+      </c>
+      <c r="U140">
+        <v>9.7992180183451724E-2</v>
+      </c>
+      <c r="V140" t="s">
+        <v>445</v>
+      </c>
+      <c r="W140" t="s">
+        <v>446</v>
+      </c>
+      <c r="X140" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y140" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="141" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="142" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>441</v>
+      </c>
+      <c r="B142">
+        <v>100</v>
+      </c>
+      <c r="C142">
+        <v>8</v>
+      </c>
+      <c r="D142">
+        <v>1E-3</v>
+      </c>
+      <c r="E142">
+        <v>0.2</v>
+      </c>
+      <c r="F142">
+        <v>0.01</v>
+      </c>
+      <c r="G142" t="s">
+        <v>449</v>
+      </c>
+      <c r="I142" t="s">
+        <v>443</v>
+      </c>
+      <c r="L142" t="s">
+        <v>443</v>
+      </c>
+      <c r="O142" t="s">
+        <v>450</v>
+      </c>
+      <c r="P142">
+        <v>0.49411764705882361</v>
+      </c>
+      <c r="Q142">
+        <v>0.45761371755179808</v>
+      </c>
+      <c r="R142">
+        <v>0.49411764705882361</v>
+      </c>
+      <c r="S142">
+        <v>0.13268203919406141</v>
+      </c>
+      <c r="T142">
+        <v>0.14378665462333939</v>
+      </c>
+      <c r="U142">
+        <v>0.13268203919406141</v>
+      </c>
+      <c r="V142" t="s">
+        <v>451</v>
+      </c>
+      <c r="W142" t="s">
+        <v>452</v>
+      </c>
+      <c r="X142" t="s">
+        <v>451</v>
+      </c>
+      <c r="Y142" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="143" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="144" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>441</v>
+      </c>
+      <c r="B144">
+        <v>100</v>
+      </c>
+      <c r="C144">
+        <v>8</v>
+      </c>
+      <c r="D144">
+        <v>1E-3</v>
+      </c>
+      <c r="E144">
+        <v>0.2</v>
+      </c>
+      <c r="F144">
+        <v>0.01</v>
+      </c>
+      <c r="G144" t="s">
+        <v>454</v>
+      </c>
+      <c r="I144" t="s">
+        <v>443</v>
+      </c>
+      <c r="L144" t="s">
+        <v>443</v>
+      </c>
+      <c r="O144" t="s">
+        <v>455</v>
+      </c>
+      <c r="P144">
+        <v>0.3411764705882353</v>
+      </c>
+      <c r="Q144">
+        <v>0.33318577191642212</v>
+      </c>
+      <c r="R144">
+        <v>0.3411764705882353</v>
+      </c>
+      <c r="S144">
+        <v>0.18905691592541149</v>
+      </c>
+      <c r="T144">
+        <v>0.18829568989524589</v>
+      </c>
+      <c r="U144">
+        <v>0.18905691592541149</v>
+      </c>
+      <c r="V144" t="s">
+        <v>456</v>
+      </c>
+      <c r="W144" t="s">
+        <v>457</v>
+      </c>
+      <c r="X144" t="s">
+        <v>456</v>
+      </c>
+      <c r="Y144" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="145" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="146" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>441</v>
+      </c>
+      <c r="B146">
+        <v>100</v>
+      </c>
+      <c r="C146">
+        <v>8</v>
+      </c>
+      <c r="D146">
+        <v>1E-3</v>
+      </c>
+      <c r="E146">
+        <v>0.2</v>
+      </c>
+      <c r="F146">
+        <v>0.01</v>
+      </c>
+      <c r="G146" t="s">
+        <v>459</v>
+      </c>
+      <c r="I146" t="s">
+        <v>443</v>
+      </c>
+      <c r="L146" t="s">
+        <v>443</v>
+      </c>
+      <c r="O146" t="s">
+        <v>460</v>
+      </c>
+      <c r="P146">
+        <v>0.3411764705882353</v>
+      </c>
+      <c r="Q146">
+        <v>0.30781455659619927</v>
+      </c>
+      <c r="R146">
+        <v>0.3411764705882353</v>
+      </c>
+      <c r="S146">
+        <v>0.1583449060198768</v>
+      </c>
+      <c r="T146">
+        <v>0.15232696511509211</v>
+      </c>
+      <c r="U146">
+        <v>0.1583449060198768</v>
+      </c>
+      <c r="V146" t="s">
+        <v>461</v>
+      </c>
+      <c r="W146" t="s">
+        <v>462</v>
+      </c>
+      <c r="X146" t="s">
+        <v>461</v>
+      </c>
+      <c r="Y146" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="148" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="149" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="150" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>441</v>
+      </c>
+      <c r="B150">
+        <v>100</v>
+      </c>
+      <c r="C150">
+        <v>8</v>
+      </c>
+      <c r="D150">
+        <v>1E-3</v>
+      </c>
+      <c r="E150">
+        <v>0.2</v>
+      </c>
+      <c r="F150">
+        <v>0.01</v>
+      </c>
+      <c r="G150" t="s">
+        <v>466</v>
+      </c>
+      <c r="I150" t="s">
+        <v>443</v>
+      </c>
+      <c r="L150" t="s">
+        <v>443</v>
+      </c>
+      <c r="O150" t="s">
+        <v>450</v>
+      </c>
+      <c r="P150">
+        <v>0.49411764705882361</v>
+      </c>
+      <c r="Q150">
+        <v>0.45761371755179808</v>
+      </c>
+      <c r="R150">
+        <v>0.49411764705882361</v>
+      </c>
+      <c r="S150">
+        <v>0.13268203919406141</v>
+      </c>
+      <c r="T150">
+        <v>0.14378665462333939</v>
+      </c>
+      <c r="U150">
+        <v>0.13268203919406141</v>
+      </c>
+      <c r="V150" t="s">
+        <v>451</v>
+      </c>
+      <c r="W150" t="s">
+        <v>452</v>
+      </c>
+      <c r="X150" t="s">
+        <v>451</v>
+      </c>
+      <c r="Y150" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="151" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="152" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>441</v>
+      </c>
+      <c r="B152">
+        <v>100</v>
+      </c>
+      <c r="C152">
+        <v>8</v>
+      </c>
+      <c r="D152">
+        <v>1E-3</v>
+      </c>
+      <c r="E152">
+        <v>0.2</v>
+      </c>
+      <c r="F152">
+        <v>0.01</v>
+      </c>
+      <c r="G152" t="s">
+        <v>467</v>
+      </c>
+      <c r="I152" t="s">
+        <v>443</v>
+      </c>
+      <c r="L152" t="s">
+        <v>443</v>
+      </c>
+      <c r="O152" t="s">
+        <v>468</v>
+      </c>
+      <c r="P152">
+        <v>0.35294117647058831</v>
+      </c>
+      <c r="Q152">
+        <v>0.329394780536649</v>
+      </c>
+      <c r="R152">
+        <v>0.35294117647058831</v>
+      </c>
+      <c r="S152">
+        <v>0.10329282742177461</v>
+      </c>
+      <c r="T152">
+        <v>8.403464523761299E-2</v>
+      </c>
+      <c r="U152">
+        <v>0.10329282742177461</v>
+      </c>
+      <c r="V152" t="s">
+        <v>469</v>
+      </c>
+      <c r="W152" t="s">
+        <v>470</v>
+      </c>
+      <c r="X152" t="s">
+        <v>469</v>
+      </c>
+      <c r="Y152" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="153" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="154" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>441</v>
+      </c>
+      <c r="B154">
+        <v>100</v>
+      </c>
+      <c r="C154">
+        <v>8</v>
+      </c>
+      <c r="D154">
+        <v>1E-3</v>
+      </c>
+      <c r="E154">
+        <v>0.2</v>
+      </c>
+      <c r="F154">
+        <v>0.01</v>
+      </c>
+      <c r="G154" t="s">
+        <v>473</v>
+      </c>
+      <c r="I154" t="s">
+        <v>443</v>
+      </c>
+      <c r="L154" t="s">
+        <v>443</v>
+      </c>
+      <c r="O154" t="s">
+        <v>450</v>
+      </c>
+      <c r="P154">
+        <v>0.49411764705882361</v>
+      </c>
+      <c r="Q154">
+        <v>0.45761371755179808</v>
+      </c>
+      <c r="R154">
+        <v>0.49411764705882361</v>
+      </c>
+      <c r="S154">
+        <v>0.13268203919406141</v>
+      </c>
+      <c r="T154">
+        <v>0.14378665462333939</v>
+      </c>
+      <c r="U154">
+        <v>0.13268203919406141</v>
+      </c>
+      <c r="V154" t="s">
+        <v>451</v>
+      </c>
+      <c r="W154" t="s">
+        <v>452</v>
+      </c>
+      <c r="X154" t="s">
+        <v>451</v>
+      </c>
+      <c r="Y154" t="s">
+        <v>453</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed F1 and Recall, added group voting metrics for majourity and average * Changed f1 and recall to be a 3 element array of the f1 and recall of the evaluated test, respectively. * Changed f1std and recallstd to include average metrics for each class, data also shows the multi-element array of the predictions * Changing the datasets of grouped2D to behave differently: ** No longer produces (# of images)*(# of desired slices) instances, it now groups the images all under a patient id ** Added evaluateGroupVoting(), which performs majourity voting based on the grouping of patients, if required, otherwise it has the same functionality as evaluate() ** Changed around getting the answer set from the testingset in evaluateModelOnTestSet()
</commit_message>
<xml_diff>
--- a/testResults.xlsx
+++ b/testResults.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnz\AppData\Local\Temp\Mxt241\RemoteFiles\656804_3_18\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnz\AppData\Local\Temp\Mxt241\RemoteFiles\67852_2_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C26A2A-8BAC-4DBC-ABE7-A0D69204D3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3BDD8B-EC39-4802-A497-2481BC1447CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6150" yWindow="1940" windowWidth="28800" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="501">
   <si>
     <t>name</t>
   </si>
@@ -1342,7 +1342,7 @@
     <t>Weight tests, viewing performance of legacy vs new weights</t>
   </si>
   <si>
-    <t>legacy weights</t>
+    <t>legacy weights, small2d</t>
   </si>
   <si>
     <t>Tests/0--/foldn5</t>
@@ -1366,7 +1366,7 @@
     <t>[14, 11, 13, 15, 15]</t>
   </si>
   <si>
-    <t>newer weights</t>
+    <t>newer weights, small2d</t>
   </si>
   <si>
     <t>python testSamples26-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='newer weights' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Small2DResnet'</t>
@@ -1384,6 +1384,9 @@
     <t>[19, 25, 35, 17, 21]</t>
   </si>
   <si>
+    <t>legacy weights, large2d</t>
+  </si>
+  <si>
     <t>python testSamples26-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='legacy weights' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Large2DResnet'</t>
   </si>
   <si>
@@ -1399,6 +1402,9 @@
     <t>[15, 15, 16, 28, 11]</t>
   </si>
   <si>
+    <t>newer weights, large2d</t>
+  </si>
+  <si>
     <t>python testSamples26-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='newer weights' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Large2DResnet'</t>
   </si>
   <si>
@@ -1414,15 +1420,18 @@
     <t>[17, 16, 18, 12, 22]</t>
   </si>
   <si>
+    <t>testing Padding on small model with tumor sizes (0 and valid padding seems to perform the same</t>
+  </si>
+  <si>
+    <t>newer weights with padding 0</t>
+  </si>
+  <si>
+    <t>python testSamples26-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='newer weights with padding 0' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Small2DResnet'</t>
+  </si>
+  <si>
     <t>newer weights with padding same</t>
   </si>
   <si>
-    <t>newer weights with padding 0</t>
-  </si>
-  <si>
-    <t>python testSamples26-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='newer weights with padding 0' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Small2DResnet'</t>
-  </si>
-  <si>
     <t>python testSamples26-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='newer weights with padding same' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Small2DResnet'</t>
   </si>
   <si>
@@ -1444,7 +1453,76 @@
     <t>python testSamples26-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='newer weights with padding valid' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Small2DResnet'</t>
   </si>
   <si>
-    <t>testing Padding on small model with tumor sizes (0 and valid padding seems to perform the same</t>
+    <t>testSamples30-7.py -- Changed f1 and recall to have multilabel scores in the std respectively. ALSO made grouped2D group patient slices togheter rather than treat each slice individually</t>
+  </si>
+  <si>
+    <t>{0: 5.2, 1: 8.0, 2: 3.8}</t>
+  </si>
+  <si>
+    <t>{0: 0.2, 1: 0.4620915032679738, 2: 0.1911111111111111}</t>
+  </si>
+  <si>
+    <t>{0: 0.22000000000000003, 1: 0.5095238095238096, 2: 0.18888888888888888}</t>
+  </si>
+  <si>
+    <t>[0.35294117647058826, 0.5294117647058824, 0.23529411764705882, 0.3333333333333333, 0.25]</t>
+  </si>
+  <si>
+    <t>[[0.0, 0.588235294117647, 0.2222222222222222], [0.5714285714285715, 0.5, 0.5333333333333333], [0.0, 0.4444444444444444, 0.0], [0.42857142857142855, 0.3333333333333333, 0.19999999999999998], [0.0, 0.4444444444444444, 0.0]]</t>
+  </si>
+  <si>
+    <t>[[0.0, 0.7142857142857143, 0.16666666666666666], [0.5, 0.42857142857142855, 0.6666666666666666], [0.0, 0.5714285714285714, 0.0], [0.6, 0.5, 0.1111111111111111], [0.0, 0.3333333333333333, 0.0]]</t>
+  </si>
+  <si>
+    <t>[17, 16, 13, 14, 28]</t>
+  </si>
+  <si>
+    <t>viewing performance on single image</t>
+  </si>
+  <si>
+    <t>python testSamples30-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='viewing performance on single image' -hasBackground=f -usesLargestBox=f -segmentsMultiple=1 -dropoutRate=0.2 -grouped2D=f -modelChosen='Small2D'</t>
+  </si>
+  <si>
+    <t>{0: 0.37222222222222223, 1: 0.6069365721997302, 2: 0.3288888888888889}</t>
+  </si>
+  <si>
+    <t>{0: 0.4, 1: 0.7035714285714285, 2: 0.2866666666666667}</t>
+  </si>
+  <si>
+    <t>[[0.0, 0.4210526315789474, 0.4444444444444445], [0.75, 0.7000000000000001, 0.33333333333333337], [0.22222222222222224, 0.6153846153846153, 0.6666666666666666], [0.4444444444444445, 0.631578947368421, 0.0], [0.4444444444444445, 0.6666666666666666, 0.2]]</t>
+  </si>
+  <si>
+    <t>[[0.0, 0.5, 0.4], [0.75, 0.875, 0.2], [0.25, 0.5714285714285714, 0.6666666666666666], [0.5, 0.8571428571428571, 0.0], [0.5, 0.7142857142857143, 0.16666666666666666]]</t>
+  </si>
+  <si>
+    <t>{0: 1.4, 1: 11.0, 2: 4.6}</t>
+  </si>
+  <si>
+    <t>{0: 0.17142857142857143, 1: 0.5678889531521111, 2: 0.3387301587301587}</t>
+  </si>
+  <si>
+    <t>{0: 0.13999999999999999, 1: 0.7571428571428571, 2: 0.36888888888888893}</t>
+  </si>
+  <si>
+    <t>[0.4117647058823529, 0.5882352941176471, 0.47058823529411764, 0.3333333333333333, 0.4375]</t>
+  </si>
+  <si>
+    <t>[[0.0, 0.631578947368421, 0.2222222222222222], [0.5714285714285715, 0.6153846153846153, 0.5714285714285715], [0.0, 0.5714285714285714, 0.5], [0.28571428571428575, 0.4210526315789474, 0.19999999999999998], [0.0, 0.6, 0.2]]</t>
+  </si>
+  <si>
+    <t>[[0.0, 0.8571428571428571, 0.16666666666666666], [0.5, 0.5714285714285714, 0.6666666666666666], [0.0, 0.8571428571428571, 0.4], [0.2, 1.0, 0.1111111111111111], [0.0, 0.5, 0.5]]</t>
+  </si>
+  <si>
+    <t>viewing performance on grouped2d majourity voting</t>
+  </si>
+  <si>
+    <t>python testSamples30-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='viewing performance on grouped2d majourity voting' -hasBackground=f -usesLargestBox=f -segmentsMultiple=13 -dropoutRate=0.2 -grouped2D=t -modelChosen='Small2D'</t>
+  </si>
+  <si>
+    <t>viewing performance on grouped2d average voting</t>
+  </si>
+  <si>
+    <t>python testSamples30-7.py -batchSize=8 -epochs=100 -lr=0.001 -evalDetailLine='viewing performance on grouped2d average voting' -hasBackground=f -usesLargestBox=f -segmentsMultiple=13 -dropoutRate=0.2 -grouped2D=t -modelChosen='Small2D'</t>
   </si>
 </sst>
 </file>
@@ -1784,10 +1862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y154"/>
+  <dimension ref="A1:Y162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A155" sqref="A155"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="N167" sqref="N167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9686,7 +9764,7 @@
     </row>
     <row r="143" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
     </row>
     <row r="144" spans="1:25" x14ac:dyDescent="0.35">
@@ -9709,7 +9787,7 @@
         <v>0.01</v>
       </c>
       <c r="G144" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="I144" t="s">
         <v>443</v>
@@ -9718,7 +9796,7 @@
         <v>443</v>
       </c>
       <c r="O144" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="P144">
         <v>0.3411764705882353</v>
@@ -9739,21 +9817,21 @@
         <v>0.18905691592541149</v>
       </c>
       <c r="V144" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="W144" t="s">
+        <v>458</v>
+      </c>
+      <c r="X144" t="s">
         <v>457</v>
       </c>
-      <c r="X144" t="s">
-        <v>456</v>
-      </c>
       <c r="Y144" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="145" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
     </row>
     <row r="146" spans="1:25" x14ac:dyDescent="0.35">
@@ -9776,7 +9854,7 @@
         <v>0.01</v>
       </c>
       <c r="G146" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="I146" t="s">
         <v>443</v>
@@ -9785,7 +9863,7 @@
         <v>443</v>
       </c>
       <c r="O146" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="P146">
         <v>0.3411764705882353</v>
@@ -9806,26 +9884,26 @@
         <v>0.1583449060198768</v>
       </c>
       <c r="V146" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="W146" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="X146" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="Y146" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="148" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
     </row>
     <row r="149" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="150" spans="1:25" x14ac:dyDescent="0.35">
@@ -9848,7 +9926,7 @@
         <v>0.01</v>
       </c>
       <c r="G150" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="I150" t="s">
         <v>443</v>
@@ -9892,7 +9970,7 @@
     </row>
     <row r="151" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
     </row>
     <row r="152" spans="1:25" x14ac:dyDescent="0.35">
@@ -9915,7 +9993,7 @@
         <v>0.01</v>
       </c>
       <c r="G152" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="I152" t="s">
         <v>443</v>
@@ -9924,7 +10002,7 @@
         <v>443</v>
       </c>
       <c r="O152" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="P152">
         <v>0.35294117647058831</v>
@@ -9945,21 +10023,21 @@
         <v>0.10329282742177461</v>
       </c>
       <c r="V152" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="W152" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="X152" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="Y152" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="153" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="154" spans="1:25" x14ac:dyDescent="0.35">
@@ -9982,7 +10060,7 @@
         <v>0.01</v>
       </c>
       <c r="G154" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="I154" t="s">
         <v>443</v>
@@ -10021,6 +10099,212 @@
         <v>451</v>
       </c>
       <c r="Y154" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="156" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="157" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="158" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>441</v>
+      </c>
+      <c r="B158">
+        <v>100</v>
+      </c>
+      <c r="C158">
+        <v>8</v>
+      </c>
+      <c r="D158">
+        <v>1E-3</v>
+      </c>
+      <c r="E158">
+        <v>0.2</v>
+      </c>
+      <c r="F158">
+        <v>0.01</v>
+      </c>
+      <c r="G158" t="s">
+        <v>498</v>
+      </c>
+      <c r="I158" t="s">
+        <v>443</v>
+      </c>
+      <c r="L158" t="s">
+        <v>443</v>
+      </c>
+      <c r="O158" t="s">
+        <v>478</v>
+      </c>
+      <c r="P158">
+        <v>0.34019607843137262</v>
+      </c>
+      <c r="Q158">
+        <v>0.284400871459695</v>
+      </c>
+      <c r="R158">
+        <v>0.30613756613756621</v>
+      </c>
+      <c r="S158">
+        <v>0.14579888192247431</v>
+      </c>
+      <c r="T158" t="s">
+        <v>479</v>
+      </c>
+      <c r="U158" t="s">
+        <v>480</v>
+      </c>
+      <c r="V158" t="s">
+        <v>481</v>
+      </c>
+      <c r="W158" t="s">
+        <v>482</v>
+      </c>
+      <c r="X158" t="s">
+        <v>483</v>
+      </c>
+      <c r="Y158" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="159" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="160" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>441</v>
+      </c>
+      <c r="B160">
+        <v>100</v>
+      </c>
+      <c r="C160">
+        <v>8</v>
+      </c>
+      <c r="D160">
+        <v>1E-3</v>
+      </c>
+      <c r="E160">
+        <v>0.2</v>
+      </c>
+      <c r="F160">
+        <v>0.01</v>
+      </c>
+      <c r="G160" t="s">
+        <v>500</v>
+      </c>
+      <c r="I160" t="s">
+        <v>443</v>
+      </c>
+      <c r="L160" t="s">
+        <v>443</v>
+      </c>
+      <c r="O160" t="s">
+        <v>491</v>
+      </c>
+      <c r="P160">
+        <v>0.44828431372549021</v>
+      </c>
+      <c r="Q160">
+        <v>0.35934922777028039</v>
+      </c>
+      <c r="R160">
+        <v>0.422010582010582</v>
+      </c>
+      <c r="S160">
+        <v>0.1157272360436034</v>
+      </c>
+      <c r="T160" t="s">
+        <v>492</v>
+      </c>
+      <c r="U160" t="s">
+        <v>493</v>
+      </c>
+      <c r="V160" t="s">
+        <v>494</v>
+      </c>
+      <c r="W160" t="s">
+        <v>495</v>
+      </c>
+      <c r="X160" t="s">
+        <v>496</v>
+      </c>
+      <c r="Y160" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="161" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="162" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>441</v>
+      </c>
+      <c r="B162">
+        <v>100</v>
+      </c>
+      <c r="C162">
+        <v>8</v>
+      </c>
+      <c r="D162">
+        <v>1E-3</v>
+      </c>
+      <c r="E162">
+        <v>0.2</v>
+      </c>
+      <c r="F162">
+        <v>0.01</v>
+      </c>
+      <c r="G162" t="s">
+        <v>486</v>
+      </c>
+      <c r="I162" t="s">
+        <v>443</v>
+      </c>
+      <c r="L162" t="s">
+        <v>443</v>
+      </c>
+      <c r="O162" t="s">
+        <v>450</v>
+      </c>
+      <c r="P162">
+        <v>0.49411764705882361</v>
+      </c>
+      <c r="Q162">
+        <v>0.43601589443694722</v>
+      </c>
+      <c r="R162">
+        <v>0.46341269841269839</v>
+      </c>
+      <c r="S162">
+        <v>0.13268203919406141</v>
+      </c>
+      <c r="T162" t="s">
+        <v>487</v>
+      </c>
+      <c r="U162" t="s">
+        <v>488</v>
+      </c>
+      <c r="V162" t="s">
+        <v>451</v>
+      </c>
+      <c r="W162" t="s">
+        <v>489</v>
+      </c>
+      <c r="X162" t="s">
+        <v>490</v>
+      </c>
+      <c r="Y162" t="s">
         <v>453</v>
       </c>
     </row>

</xml_diff>